<commit_message>
added admin & user change passsword and account settings
</commit_message>
<xml_diff>
--- a/assets/docs/members_list.xlsx
+++ b/assets/docs/members_list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
     <t>ID</t>
   </si>
@@ -30,24 +30,6 @@
   </si>
   <si>
     <t>PHONE</t>
-  </si>
-  <si>
-    <t>Debajyoti Das</t>
-  </si>
-  <si>
-    <t>sidart101@gmail.com</t>
-  </si>
-  <si>
-    <t>web wizard</t>
-  </si>
-  <si>
-    <t>91-3872446878</t>
-  </si>
-  <si>
-    <t>Sifhi if aioheifhai</t>
-  </si>
-  <si>
-    <t>sid94.dev@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -386,7 +368,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -411,36 +393,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3"/>
-      <c r="E3"/>
-    </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>

</xml_diff>